<commit_message>
setting karyawan has done
</commit_message>
<xml_diff>
--- a/public/user.xlsx
+++ b/public/user.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="DAFTAR_DAFTAR" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,18 +21,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
-  <si>
-    <t xml:space="preserve">fullname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">initial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birth_date</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="141">
+  <si>
+    <t xml:space="preserve">nik (sebagai acuan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nama_lengkap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nama_panggilan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inisial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tanggal_lahir</t>
   </si>
   <si>
     <t xml:space="preserve">alamat</t>
@@ -41,7 +44,10 @@
     <t xml:space="preserve">no_telp</t>
   </si>
   <si>
-    <t xml:space="preserve">email</t>
+    <t xml:space="preserve">email_pribadi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email_kantor</t>
   </si>
   <si>
     <t xml:space="preserve">username</t>
@@ -59,43 +65,73 @@
     <t xml:space="preserve">nik_evaluator_2</t>
   </si>
   <si>
+    <t xml:space="preserve">divisi</t>
+  </si>
+  <si>
     <t xml:space="preserve">posisi</t>
   </si>
   <si>
     <t xml:space="preserve">sisa_cuti</t>
   </si>
   <si>
-    <t xml:space="preserve">action</t>
+    <t xml:space="preserve">status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tanggal_gabung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tanggal_mulai_cuti_besar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sisa_cuti_besar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tanggal_frame_berikutnya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tanggal_lensa_berikutnya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01234</t>
   </si>
   <si>
     <t xml:space="preserve">Nama Lengkap</t>
   </si>
   <si>
+    <t xml:space="preserve">Nama</t>
+  </si>
+  <si>
     <t xml:space="preserve">NL</t>
   </si>
   <si>
-    <t xml:space="preserve">01234</t>
-  </si>
-  <si>
     <t xml:space="preserve">02123456</t>
   </si>
   <si>
     <t xml:space="preserve">nl@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">nl@polagroup.co.id</t>
+  </si>
+  <si>
     <t xml:space="preserve">P40</t>
   </si>
   <si>
     <t xml:space="preserve">PIP</t>
   </si>
   <si>
-    <t xml:space="preserve">00123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CREATE</t>
+    <t xml:space="preserve">02828</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02822</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board Of Director</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tetap</t>
   </si>
   <si>
     <t xml:space="preserve">SUBSDIARY</t>
@@ -273,6 +309,141 @@
   </si>
   <si>
     <t xml:space="preserve">Pola Megafit Indonesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List Building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grha Essi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPW Cikupa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RDO Jl Panjang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPE Pangjay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPW PGA Ceger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAP Puri Niaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAP SMI Kedoya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDYN Aries Niaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PGP Kebun Jeruk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPE Taman Tekno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PGP Taman Tekno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPW Taman Tekno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAP Gatot Subroto Bandung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPW Metro Trade Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDYN Ruko CBD Sukaraja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPE PL Bandung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAP Lippo Industrial Esate Bekasi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDYN Grand Galaxy City Bekasi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAP Bekasi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDYN Karanganyar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAP Karanganyar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPW Kawasan Industri Tugu Semarang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAP Komp Mutiara Marina 19 Semarang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPW PGA Pandaan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAP Surabaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPW Bali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDYN Sidoarjo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAP Batam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPW Batam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAP PDYN Medan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPW Medan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPW Palembang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAP Palembang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDYN Riau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAP Pekanbaru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPW Pekanbaru </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPE Pekanbaru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPE Balikpapan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PGP Balikpapan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPW Balikpapan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPE Bontang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAP Banjarbaru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPW Banjarbaru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPW Makassar</t>
   </si>
 </sst>
 </file>
@@ -283,7 +454,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -309,13 +480,6 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -375,8 +539,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -388,11 +556,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -400,12 +564,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -485,19 +653,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.32"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="20.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="14.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="22.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="22.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="22.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="24" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -546,79 +727,116 @@
       <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="n">
         <v>43882</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>4</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="4" t="n">
-        <v>99999</v>
+        <v>29</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>30</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>24</v>
+      <c r="R2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="2" t="n">
+        <v>42139</v>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>44216</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="V2" s="4" t="n">
+        <v>44185</v>
+      </c>
+      <c r="W2" s="4" t="n">
+        <v>44185</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2" type="list">
-      <formula1>"BPW,PSP,PGP,PIP,PGA,BKW,PARP,PRA,PSA,DPE,IPL,PPE,PMP,PL,IM,PAI,TPP,TPF,PBP,PCP,PPC,RDO,PMP,EPU,EG,PEP,PAP,PRD,SMI,PMI"</formula1>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q2" type="none">
+      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="list">
-      <formula1>"CREATE,UPDATE,DELETE"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
-      <formula1>"Account Payable,Account Receviable,Accounting,Admin,Admin AE,Admin Marketing,Admin Procurement,Admin Project Sales  Rental,Admin Project Service,Admin Report PSV,Auditor,Building Maintenance Staff,Cashier,Chief Operating Officer,Cleaning,Collector,Comben"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2" type="list">
-      <formula1>"P40,Grha Essi,BPW Cikupa,RDO Jl Panjang,DPE Pangjay,BPW PGA Ceger,PAP Puri Niaga,PAP SMI Kedoya,PDYN Aries Niaga,PGP Jl Raya Pos Pengumben,PPE Taman Tekno,PGP Taman Tekno,BPW Taman Tekno,EPU Pergudangan Perum,PAP Gatot Subroto Bandung,BPW Metro Trade Cent"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="none">
-      <formula1>0</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R2" type="list">
+      <formula1>"Tetap,Kontrak,Probation"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="nl@gmail.com"/>
+    <hyperlink ref="H2" r:id="rId1" display="nl@gmail.com"/>
+    <hyperlink ref="I2" r:id="rId2" display="nl@polagroup.co.id"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -635,262 +853,492 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>83</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="8" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug has done
</commit_message>
<xml_diff>
--- a/public/user.xlsx
+++ b/public/user.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="137">
   <si>
     <t xml:space="preserve">nik (sebagai acuan)</t>
   </si>
@@ -65,12 +65,6 @@
     <t xml:space="preserve">nik_evaluator_2</t>
   </si>
   <si>
-    <t xml:space="preserve">divisi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">posisi</t>
-  </si>
-  <si>
     <t xml:space="preserve">sisa_cuti</t>
   </si>
   <si>
@@ -123,12 +117,6 @@
   </si>
   <si>
     <t xml:space="preserve">02822</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Board Of Director</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software Engineer</t>
   </si>
   <si>
     <t xml:space="preserve">Tetap</t>
@@ -653,15 +641,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="11.52"/>
@@ -671,14 +659,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.92"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="20.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="14.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="22.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="22.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="22.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="22.49"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="24" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="22.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -742,28 +729,22 @@
       <c r="T1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="V1" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>43882</v>
@@ -772,64 +753,58 @@
         <v>5</v>
       </c>
       <c r="G2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="N2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="O2" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="2" t="n">
+      <c r="Q2" s="2" t="n">
         <v>42139</v>
       </c>
-      <c r="T2" s="2" t="n">
+      <c r="R2" s="2" t="n">
         <v>44216</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="S2" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="V2" s="4" t="n">
+      <c r="T2" s="4" t="n">
         <v>44185</v>
       </c>
-      <c r="W2" s="4" t="n">
+      <c r="U2" s="4" t="n">
         <v>44185</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q2" type="none">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2" type="list">
       <formula1>"Tetap,Kontrak,Probation"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -868,477 +843,477 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>